<commit_message>
25 shipped compounds to DLS team for soaking
</commit_message>
<xml_diff>
--- a/New folder/April2025-NSP3-MD.xlsx
+++ b/New folder/April2025-NSP3-MD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadia\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE14564-3486-4143-9AAB-B4D3343C7FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6893C1AB-1E40-44A0-B900-C8C5B855C53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B085EE33-547E-4087-9145-EB3CEE4BA804}"/>
   </bookViews>
@@ -385,7 +385,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +417,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -444,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,6 +475,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,7 +816,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1265,7 +1275,7 @@
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1295,7 +1305,7 @@
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1325,7 +1335,7 @@
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1355,7 +1365,7 @@
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1385,7 +1395,7 @@
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1415,7 +1425,7 @@
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1445,7 +1455,7 @@
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1475,7 +1485,7 @@
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1505,7 +1515,7 @@
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="10" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1535,7 +1545,7 @@
       <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1565,7 +1575,7 @@
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="3" t="s">

</xml_diff>